<commit_message>
Added links to Services
</commit_message>
<xml_diff>
--- a/AWS_Products.xlsx
+++ b/AWS_Products.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/Desktop/United/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsarma/git/github/palsarma/aws_products/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="269">
   <si>
     <t>Category</t>
   </si>
@@ -831,13 +831,16 @@
   </si>
   <si>
     <t>A Free Cross-Platform 3D Game Engine with Full Source, Integrated with AWS and Twitch</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -848,6 +851,14 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -870,20 +881,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -957,12 +988,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C132" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:C132"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Category" dataDxfId="4"/>
-    <tableColumn id="2" name="AWS Service" dataDxfId="3"/>
-    <tableColumn id="3" name="Description" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D132" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D132"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Category" dataDxfId="3"/>
+    <tableColumn id="3" name="AWS Service" dataDxfId="2"/>
+    <tableColumn id="4" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" name="Link" dataDxfId="0" dataCellStyle="Hyperlink">
+      <calculatedColumnFormula>HYPERLINK(Table2[[#This Row],[Link]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1231,21 +1265,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="54" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,8 +1288,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1266,8 +1302,12 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ec2/?p=tile</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1277,8 +1317,12 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ec2/autoscaling/?p=tile</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1288,8 +1332,12 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ecs/?p=tile</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1299,8 +1347,12 @@
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/eks/?p=tile</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1310,8 +1362,12 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ecr/?p=tile</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1321,8 +1377,12 @@
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/lightsail/?p=tile</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1332,8 +1392,12 @@
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/batch/?p=tile</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1343,8 +1407,12 @@
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elasticbeanstalk/?p=tile</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1354,8 +1422,12 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/fargate/?p=tile</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -1365,8 +1437,12 @@
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/lambda/?p=tile</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1376,8 +1452,12 @@
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/serverless/serverlessrepo/?p=tile</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1387,8 +1467,12 @@
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/vmware/?p=tile</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1398,8 +1482,12 @@
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/s3/?p=tile</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1409,8 +1497,12 @@
       <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ebs/?p=tile</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1420,8 +1512,12 @@
       <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/efs/?p=tile</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1431,8 +1527,12 @@
       <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/glacier1/?p=tile</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1442,8 +1542,12 @@
       <c r="C18" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/storagegateway/?p=tile</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1453,8 +1557,12 @@
       <c r="C19" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowball/?p=tile</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1464,8 +1572,12 @@
       <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
@@ -1475,8 +1587,12 @@
       <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1486,8 +1602,12 @@
       <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/rds/aurora/?p=tile</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1497,8 +1617,12 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/rds/?p=tile</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1508,8 +1632,12 @@
       <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/dynamodb/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1519,8 +1647,12 @@
       <c r="C25" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elasticache/?p=tile</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1530,8 +1662,12 @@
       <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/redshift/?p=tile</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1541,8 +1677,12 @@
       <c r="C27" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/neptune/?p=tile</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
@@ -1552,8 +1692,12 @@
       <c r="C28" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/dms/?p=tile</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1563,8 +1707,12 @@
       <c r="C29" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/application-discovery/?p=tile</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1574,8 +1722,12 @@
       <c r="C30" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/dms/?p=tile</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1585,8 +1737,12 @@
       <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/migration-hub/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1596,8 +1752,12 @@
       <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/server-migration-service/?p=tile</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -1607,8 +1767,12 @@
       <c r="C33" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowball/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -1618,8 +1782,12 @@
       <c r="C34" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowball-edge/?p=tile</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>60</v>
       </c>
@@ -1629,8 +1797,12 @@
       <c r="C35" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/snowmobile/?p=tile</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -1640,8 +1812,12 @@
       <c r="C36" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/vpc/?p=tile</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
@@ -1651,8 +1827,12 @@
       <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudfront/?p=tile</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>67</v>
       </c>
@@ -1662,8 +1842,12 @@
       <c r="C38" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/route53/?p=tile</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>67</v>
       </c>
@@ -1673,8 +1857,12 @@
       <c r="C39" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>67</v>
       </c>
@@ -1684,8 +1872,12 @@
       <c r="C40" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/directconnect/?p=tile</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
@@ -1695,8 +1887,12 @@
       <c r="C41" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elasticloadbalancing/?p=tile</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -1706,8 +1902,12 @@
       <c r="C42" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/codestar/?p=tile</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -1717,8 +1917,12 @@
       <c r="C43" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/codecommit/?p=tile</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>80</v>
       </c>
@@ -1728,8 +1932,12 @@
       <c r="C44" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/codebuild/?p=tile</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>80</v>
       </c>
@@ -1739,8 +1947,12 @@
       <c r="C45" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/codedeploy/?p=tile</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>80</v>
       </c>
@@ -1750,8 +1962,12 @@
       <c r="C46" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/codepipeline/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>80</v>
       </c>
@@ -1761,8 +1977,12 @@
       <c r="C47" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloud9/?p=tile</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>80</v>
       </c>
@@ -1772,8 +1992,12 @@
       <c r="C48" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/xray/?p=tile</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
@@ -1783,8 +2007,12 @@
       <c r="C49" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cli/?p=tile</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
@@ -1794,8 +2022,12 @@
       <c r="C50" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudwatch/?p=tile</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
@@ -1805,8 +2037,12 @@
       <c r="C51" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/autoscaling/?p=tile</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>97</v>
       </c>
@@ -1816,8 +2052,12 @@
       <c r="C52" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudformation/?p=tile</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>97</v>
       </c>
@@ -1827,8 +2067,12 @@
       <c r="C53" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudtrail/?p=tile</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>97</v>
       </c>
@@ -1838,8 +2082,12 @@
       <c r="C54" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/config/?p=tile</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>97</v>
       </c>
@@ -1849,8 +2097,12 @@
       <c r="C55" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/opsworks/?p=tile</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>97</v>
       </c>
@@ -1860,8 +2112,12 @@
       <c r="C56" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/servicecatalog/?p=tile</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -1871,8 +2127,12 @@
       <c r="C57" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/systems-manager/?p=tile</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>97</v>
       </c>
@@ -1882,8 +2142,12 @@
       <c r="C58" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/trustedadvisor/?p=tile</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>97</v>
       </c>
@@ -1893,8 +2157,12 @@
       <c r="C59" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/premiumsupport/phd/?p=tile</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
@@ -1904,8 +2172,12 @@
       <c r="C60" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elastictranscoder/?p=tile</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>118</v>
       </c>
@@ -1915,8 +2187,12 @@
       <c r="C61" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/kinesis/video-streams/?p=tile</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -1926,8 +2202,12 @@
       <c r="C62" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mediaconvert/?p=tile</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>118</v>
       </c>
@@ -1937,8 +2217,12 @@
       <c r="C63" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/medialive/?p=tile</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>118</v>
       </c>
@@ -1948,8 +2232,12 @@
       <c r="C64" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mediapackage/?p=tile</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>118</v>
       </c>
@@ -1959,8 +2247,12 @@
       <c r="C65" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mediastore/?p=tile</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>118</v>
       </c>
@@ -1970,8 +2262,12 @@
       <c r="C66" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mediatailor/?p=tile</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
@@ -1981,8 +2277,12 @@
       <c r="C67" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iam/?p=tile</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>133</v>
       </c>
@@ -1992,8 +2292,12 @@
       <c r="C68" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloud-directory/?p=tile</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
@@ -2003,8 +2307,12 @@
       <c r="C69" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cognito/?p=tile</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>133</v>
       </c>
@@ -2014,8 +2322,12 @@
       <c r="C70" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/single-sign-on/?p=tile</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>133</v>
       </c>
@@ -2025,8 +2337,12 @@
       <c r="C71" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/guardduty/?p=tile</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>133</v>
       </c>
@@ -2036,8 +2352,12 @@
       <c r="C72" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/directconnect/?p=tile</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>133</v>
       </c>
@@ -2047,8 +2367,12 @@
       <c r="C73" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/inspector/?p=tile</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>133</v>
       </c>
@@ -2058,8 +2382,12 @@
       <c r="C74" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/macie/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
@@ -2069,8 +2397,12 @@
       <c r="C75" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/certificate-manager/?p=tile</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>133</v>
       </c>
@@ -2080,8 +2412,12 @@
       <c r="C76" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudhsm/?p=tile</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>133</v>
       </c>
@@ -2091,8 +2427,12 @@
       <c r="C77" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/directoryservice/?p=tile</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>133</v>
       </c>
@@ -2102,8 +2442,12 @@
       <c r="C78" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/kms/?p=tile</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>133</v>
       </c>
@@ -2113,8 +2457,12 @@
       <c r="C79" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/organizations/?p=tile</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>133</v>
       </c>
@@ -2124,8 +2472,12 @@
       <c r="C80" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/shield/?p=tile</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>133</v>
       </c>
@@ -2135,8 +2487,12 @@
       <c r="C81" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/waf/?p=tile</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2146,8 +2502,12 @@
       <c r="C82" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/athena/?p=tile</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>162</v>
       </c>
@@ -2157,8 +2517,12 @@
       <c r="C83" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elasticmapreduce/?p=tile</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>162</v>
       </c>
@@ -2168,8 +2532,12 @@
       <c r="C84" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/cloudsearch/?p=tile</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>162</v>
       </c>
@@ -2179,8 +2547,12 @@
       <c r="C85" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/elasticsearch-service/?p=tile</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>162</v>
       </c>
@@ -2190,8 +2562,12 @@
       <c r="C86" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/kinesis/?p=tile</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>162</v>
       </c>
@@ -2201,8 +2577,12 @@
       <c r="C87" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/redshift/?p=tile</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>162</v>
       </c>
@@ -2212,8 +2592,12 @@
       <c r="C88" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/quicksight/?p=tile</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>162</v>
       </c>
@@ -2223,8 +2607,12 @@
       <c r="C89" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/datapipeline/?p=tile</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>162</v>
       </c>
@@ -2234,8 +2622,12 @@
       <c r="C90" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/glue/?p=tile</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>179</v>
       </c>
@@ -2245,8 +2637,12 @@
       <c r="C91" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/sagemaker/?p=tile</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>179</v>
       </c>
@@ -2256,8 +2652,12 @@
       <c r="C92" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/comprehend/?p=tile</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>179</v>
       </c>
@@ -2267,8 +2667,12 @@
       <c r="C93" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/lex/?p=tile</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>179</v>
       </c>
@@ -2278,8 +2682,12 @@
       <c r="C94" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/polly/?p=tile</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>179</v>
       </c>
@@ -2289,8 +2697,12 @@
       <c r="C95" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/rekognition/?p=tile</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>179</v>
       </c>
@@ -2300,8 +2712,12 @@
       <c r="C96" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/machine-learning/?p=tile</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>179</v>
       </c>
@@ -2311,8 +2727,12 @@
       <c r="C97" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/translate/?p=tile</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>179</v>
       </c>
@@ -2322,8 +2742,12 @@
       <c r="C98" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/transcribe/?p=tile</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>179</v>
       </c>
@@ -2333,8 +2757,12 @@
       <c r="C99" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/deeplens/?p=tile</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>179</v>
       </c>
@@ -2344,8 +2772,12 @@
       <c r="C100" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/amazon-ai/amis/?p=tile</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>179</v>
       </c>
@@ -2355,8 +2787,12 @@
       <c r="C101" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mxnet/?p=tile</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>179</v>
       </c>
@@ -2366,8 +2802,12 @@
       <c r="C102" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/tensorflow/?p=tile</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
@@ -2377,8 +2817,12 @@
       <c r="C103" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mobile/?p=tile</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>204</v>
       </c>
@@ -2388,8 +2832,12 @@
       <c r="C104" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/api-gateway/?p=tile</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>204</v>
       </c>
@@ -2399,8 +2847,12 @@
       <c r="C105" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>204</v>
       </c>
@@ -2410,8 +2862,12 @@
       <c r="C106" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/appsync/?p=tile</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>204</v>
       </c>
@@ -2421,8 +2877,12 @@
       <c r="C107" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/device-farm/?p=tile</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>204</v>
       </c>
@@ -2432,8 +2892,12 @@
       <c r="C108" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/mobile/sdk/?p=tile</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>215</v>
       </c>
@@ -2443,8 +2907,12 @@
       <c r="C109" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/sumerian/?p=tile</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>218</v>
       </c>
@@ -2454,8 +2922,12 @@
       <c r="C110" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/step-functions/?p=tile</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>218</v>
       </c>
@@ -2465,8 +2937,12 @@
       <c r="C111" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/sqs/?p=tile</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>218</v>
       </c>
@@ -2476,8 +2952,12 @@
       <c r="C112" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/sns/?p=tile</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>218</v>
       </c>
@@ -2487,8 +2967,12 @@
       <c r="C113" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/amazon-mq/?p=tile</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>227</v>
       </c>
@@ -2498,8 +2982,12 @@
       <c r="C114" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/connect/?p=tile</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>227</v>
       </c>
@@ -2509,8 +2997,12 @@
       <c r="C115" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/pinpoint/?p=tile</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>227</v>
       </c>
@@ -2520,8 +3012,12 @@
       <c r="C116" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/ses/?p=tile</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>232</v>
       </c>
@@ -2531,8 +3027,12 @@
       <c r="C117" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/alexaforbusiness/?p=tile</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>232</v>
       </c>
@@ -2542,8 +3042,12 @@
       <c r="C118" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/chime/?p=tile</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>232</v>
       </c>
@@ -2553,8 +3057,12 @@
       <c r="C119" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/workdocs/?p=tile</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>232</v>
       </c>
@@ -2564,8 +3072,12 @@
       <c r="C120" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/workmail/?p=tile</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>241</v>
       </c>
@@ -2575,8 +3087,12 @@
       <c r="C121" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/workspaces/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>241</v>
       </c>
@@ -2586,8 +3102,12 @@
       <c r="C122" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/appstream2/?hp=tile&amp;so-exp=below</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>246</v>
       </c>
@@ -2597,8 +3117,12 @@
       <c r="C123" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot-core/?p=tile</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>246</v>
       </c>
@@ -2608,8 +3132,12 @@
       <c r="C124" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/freertos/?p=tile</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>246</v>
       </c>
@@ -2619,8 +3147,12 @@
       <c r="C125" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/greengrass/?p=tile</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>246</v>
       </c>
@@ -2630,8 +3162,12 @@
       <c r="C126" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot-1-click/button/?p=tile</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>246</v>
       </c>
@@ -2641,8 +3177,12 @@
       <c r="C127" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot-analytics/?p=tile</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>246</v>
       </c>
@@ -2652,8 +3192,12 @@
       <c r="C128" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot/button/?p=tile</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>246</v>
       </c>
@@ -2663,8 +3207,12 @@
       <c r="C129" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot-device-defender/?p=tile</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>246</v>
       </c>
@@ -2674,8 +3222,12 @@
       <c r="C130" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/iot-device-management/?p=tile</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>263</v>
       </c>
@@ -2685,8 +3237,12 @@
       <c r="C131" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/gamelift/?p=tile</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>263</v>
       </c>
@@ -2695,6 +3251,10 @@
       </c>
       <c r="C132" s="1" t="s">
         <v>267</v>
+      </c>
+      <c r="D132" s="2" t="str">
+        <f ca="1">HYPERLINK(Table2[[#This Row],[Link]])</f>
+        <v>https://aws.amazon.com/lumberyard/?p=tile</v>
       </c>
     </row>
   </sheetData>

</xml_diff>